<commit_message>
Updated ISL model - 2025-08-01 01:17
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/SuppXLS/scen_tsparameters_ts_108.xlsx
+++ b/VerveStacks_ISL/SuppXLS/scen_tsparameters_ts_108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ISL\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AADEAF1-A839-4526-8D50-3401BE04E2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0C175E-9789-45F4-94BF-99A7F59BC293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -927,10 +927,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>TaD,Wb0122h12,Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h08,Tc0917h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h12,Wb0121h13,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,RaD,Wb0122h11,Wb0122h15,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h10,Tc0917h14,Wb0121h14,Wb0121h16</t>
-  </si>
-  <si>
-    <t>RaN,Tc0917h20,Wb0122h20,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,Tc0917h23,Wb0121h02,Wb0121h06,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,SaP,Tc0916h06,Tc0917h01,Tc0916h04,Tc0917h24,TaN,Tc0916h03,Tc0916h23,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0917h02,Tc0917h06,WaP,Wb0122h22</t>
+    <t>Tc0916h11,Wb0121h09,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,RaD,Wb0122h11,Wb0122h15,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Wb0121h14,Wb0121h16,Wb0121h13,Tc0917h08,Tc0917h17,Tc0916h10,Tc0917h14,TaD,Wb0122h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h12,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17</t>
+  </si>
+  <si>
+    <t>TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h04,SaP,Tc0916h06,Tc0917h01,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h02,Tc0917h06,WaP,Wb0122h22,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaN,Tc0917h20,Wb0122h20,TaN,Tc0916h03,Tc0916h23,Wb0121h05,Wb0121h24,Tc0917h23,Wb0121h02,Wb0121h06,Tc0917h24,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1498,7 +1498,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>RaN,Tc0917h20,Wb0122h20,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,Tc0917h23,Wb0121h02,Wb0121h06,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,SaP,Tc0916h06,Tc0917h01,Tc0916h04,Tc0917h24,TaN,Tc0916h03,Tc0916h23,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0917h02,Tc0917h06,WaP,Wb0122h22</v>
+        <v>TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h04,SaP,Tc0916h06,Tc0917h01,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h02,Tc0917h06,WaP,Wb0122h22,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaN,Tc0917h20,Wb0122h20,TaN,Tc0916h03,Tc0916h23,Wb0121h05,Wb0121h24,Tc0917h23,Wb0121h02,Wb0121h06,Tc0917h24,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>TaD,Wb0122h12,Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h08,Tc0917h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h12,Wb0121h13,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,RaD,Wb0122h11,Wb0122h15,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h10,Tc0917h14,Wb0121h14,Wb0121h16</v>
+        <v>Tc0916h11,Wb0121h09,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,RaD,Wb0122h11,Wb0122h15,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Wb0121h14,Wb0121h16,Wb0121h13,Tc0917h08,Tc0917h17,Tc0916h10,Tc0917h14,TaD,Wb0122h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h12,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2143,7 +2143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5347852B-418B-4120-81B0-76530D082CC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBF4715-14BC-4E9E-892F-1C299021F4AC}">
   <dimension ref="B2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3288,7 +3288,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E85398B-36B1-47D9-9086-F2EEECC54B5C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0CF0EE-50DF-45BC-9BB8-D375C8F57BC7}">
   <dimension ref="B2:O111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6155,7 +6155,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D10E06-FBDC-469D-B6D3-4AC5FC3039C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCFDD8F7-A35E-43BF-974B-744104E49BFE}">
   <dimension ref="B2:O211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>